<commit_message>
Changes made to documentation
</commit_message>
<xml_diff>
--- a/documentation/testplan.xlsx
+++ b/documentation/testplan.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14128"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Timothy\Desktop\ict207project\documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="8250"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20415" windowHeight="3075"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -123,6 +128,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -137,7 +145,7 @@
     <tableColumn id="4" name="Expected Output"/>
     <tableColumn id="5" name="Passed"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -184,7 +192,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -219,7 +227,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -432,7 +440,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>